<commit_message>
[12.0][FIX] move ref on excel
</commit_message>
<xml_diff>
--- a/altinkaya_excel_export/export_account_move_line_xlsx/move_lines.xlsx
+++ b/altinkaya_excel_export/export_account_move_line_xlsx/move_lines.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Yevmiye</t>
   </si>
   <si>
-    <t xml:space="preserve">Yevmiye Referansı</t>
+    <t xml:space="preserve">Açıklama</t>
   </si>
   <si>
     <t xml:space="preserve">Cari Adi</t>
@@ -188,14 +188,14 @@
   <dimension ref="A1:HT1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="50.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.86"/>

</xml_diff>